<commit_message>
json for works in series
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E52A5C-D2BF-3244-A988-F54D9C9E138C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18252E2D-5071-4A4D-A946-DB738F2AC2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="6" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
+    <workbookView xWindow="-20" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
@@ -1581,11 +1581,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A006D3C4-93E9-0943-8732-0CF384DB2AB6}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -4309,7 +4309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D2348F-09E6-1C4F-A712-D75D02A09D8F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
updated schema to reflect change from attachments to files
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,19 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C33C27-35C3-5F4C-BDFC-84B50007EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C074FA76-5BB0-0D4C-BBEF-DA9AA15C5CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="2" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
     <sheet name="Works" sheetId="2" r:id="rId2"/>
     <sheet name="WorkFiles" sheetId="10" r:id="rId3"/>
-    <sheet name="WorkAttachments" sheetId="5" r:id="rId4"/>
-    <sheet name="Series" sheetId="9" r:id="rId5"/>
-    <sheet name="Themes" sheetId="6" r:id="rId6"/>
-    <sheet name="ThemeSeries" sheetId="7" r:id="rId7"/>
-    <sheet name="lookups" sheetId="4" r:id="rId8"/>
+    <sheet name="Series" sheetId="9" r:id="rId4"/>
+    <sheet name="Themes" sheetId="6" r:id="rId5"/>
+    <sheet name="ThemeSeries" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="162">
   <si>
     <t>Column name</t>
   </si>
@@ -87,18 +85,6 @@
     <t>checksum</t>
   </si>
   <si>
-    <t>image_id</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>caption</t>
-  </si>
-  <si>
     <t>year_display</t>
   </si>
   <si>
@@ -120,30 +106,15 @@
     <t>duration</t>
   </si>
   <si>
-    <t>optional, short</t>
-  </si>
-  <si>
-    <t>supplementary images</t>
-  </si>
-  <si>
     <t>master table (one row per work)</t>
   </si>
   <si>
-    <t>WorkImages</t>
-  </si>
-  <si>
     <t>Works</t>
   </si>
   <si>
     <t>in table</t>
   </si>
   <si>
-    <t>Works.tags</t>
-  </si>
-  <si>
-    <t>WorkImages.role</t>
-  </si>
-  <si>
     <t>physical dimensions</t>
   </si>
   <si>
@@ -228,30 +199,6 @@
     <t>for work item description</t>
   </si>
   <si>
-    <t>join supplemental images to a work page.</t>
-  </si>
-  <si>
-    <t>not derived from other fields, leave work-specific and follow master image naming</t>
-  </si>
-  <si>
-    <t>context to detail / wip images.</t>
-  </si>
-  <si>
-    <t>progress timeline context if available</t>
-  </si>
-  <si>
-    <t>image_date</t>
-  </si>
-  <si>
-    <t>internal-only notes (not exported)</t>
-  </si>
-  <si>
-    <t>admin commentary and process notes.</t>
-  </si>
-  <si>
-    <t>optional date e.g. WIP date</t>
-  </si>
-  <si>
     <t>supports curated groupings and 'more in this series'</t>
   </si>
   <si>
@@ -273,18 +220,12 @@
     <t>medium_caption</t>
   </si>
   <si>
-    <t>Works.medium_type</t>
-  </si>
-  <si>
     <t>yes - in cell list</t>
   </si>
   <si>
     <t>yes - lookup list</t>
   </si>
   <si>
-    <t>Works.storage_location</t>
-  </si>
-  <si>
     <t>for reference only - lookup list</t>
   </si>
   <si>
@@ -297,15 +238,6 @@
     <t>curve poems</t>
   </si>
   <si>
-    <t>alt</t>
-  </si>
-  <si>
-    <t>alt description e.g. 'Detail of work 00286'</t>
-  </si>
-  <si>
-    <t>accessibility</t>
-  </si>
-  <si>
     <t>public label</t>
   </si>
   <si>
@@ -333,54 +265,21 @@
     <t>curves;intuition</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>reference for image rows; debugging, curation, sorting</t>
-  </si>
-  <si>
     <t>00286-work-card.pdf</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
     <t>work card (PDF)</t>
   </si>
   <si>
-    <t>WorkAttachments</t>
-  </si>
-  <si>
     <t>file downloads</t>
   </si>
   <si>
     <t>e.g. 'work card (PDF)'</t>
   </si>
   <si>
-    <t>list label</t>
-  </si>
-  <si>
-    <t>attachment_id</t>
-  </si>
-  <si>
-    <t>file name in the scope of the work item</t>
-  </si>
-  <si>
-    <t>ID for the attachment file e.g. 001</t>
-  </si>
-  <si>
-    <t>ID for the image record e.g. 001</t>
-  </si>
-  <si>
     <t>sequential ID (e.g. 00286), text</t>
   </si>
   <si>
-    <t>filename e.g. 00286-detail-001.webp</t>
-  </si>
-  <si>
-    <t>file name e.g. '00286-work-card.pdf' (all file types are treated as 'attachments')</t>
-  </si>
-  <si>
     <t>pencil and ink on paper</t>
   </si>
   <si>
@@ -612,16 +511,22 @@
     <t>curves</t>
   </si>
   <si>
-    <t>detail | work in progress | installation</t>
-  </si>
-  <si>
-    <t>consistent meaning and optional grouping of images on the work page.</t>
-  </si>
-  <si>
     <t>file_id</t>
   </si>
   <si>
     <t>file_label</t>
+  </si>
+  <si>
+    <t>WorkFiles</t>
+  </si>
+  <si>
+    <t>file name e.g. '00286-work-card.pdf'</t>
+  </si>
+  <si>
+    <t>used for link text</t>
+  </si>
+  <si>
+    <t>used to derive link url</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +932,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -1044,23 +949,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>1</v>
@@ -1078,10 +983,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1090,13 +995,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1108,10 +1013,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1123,10 +1028,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1135,13 +1040,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1153,10 +1058,10 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1165,16 +1070,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1183,13 +1088,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1198,13 +1103,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1213,13 +1118,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1228,13 +1133,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1243,13 +1148,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1261,13 +1166,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1276,13 +1181,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1294,13 +1199,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1309,16 +1214,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1333,7 +1238,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1345,10 +1250,10 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1363,204 +1268,62 @@
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B26,#REF!,1,FALSE)))</f>
-        <v>0</v>
+        <f>NOT(ISERROR(HLOOKUP(B26,WorkFiles!$1:$1,1,FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B27,#REF!,1,FALSE)))</f>
-        <v>0</v>
+        <f>NOT(ISERROR(HLOOKUP(B27,WorkFiles!$1:$1,1,FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>3</v>
+        <v>156</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>61</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B28,#REF!,1,FALSE)))</f>
-        <v>0</v>
+        <f>NOT(ISERROR(HLOOKUP(B28,WorkFiles!$1:$1,1,FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>157</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>189</v>
+        <v>77</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B29,#REF!,1,FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B30,#REF!,1,FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B31,#REF!,1,FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B32,#REF!,1,FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B33,#REF!,1,FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B37,WorkAttachments!$1:$1,1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B38,WorkAttachments!$1:$1,1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B39,WorkAttachments!$1:$1,1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B40,WorkAttachments!$1:$1,1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>104</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1572,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A006D3C4-93E9-0943-8732-0CF384DB2AB6}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1600,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
@@ -1609,40 +1372,40 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>11</v>
@@ -1653,13 +1416,13 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1">
         <v>2024</v>
@@ -1668,16 +1431,16 @@
         <v>2024</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K2" s="1">
         <v>42</v>
@@ -1686,24 +1449,24 @@
         <v>29.7</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O2" s="8">
         <v>46046</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1">
         <v>2024</v>
@@ -1712,16 +1475,16 @@
         <v>2024</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="K3" s="1">
         <v>29.7</v>
@@ -1730,24 +1493,24 @@
         <v>42</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O3" s="8">
         <v>46046</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1">
         <v>2024</v>
@@ -1756,16 +1519,16 @@
         <v>2024</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K4" s="1">
         <v>42</v>
@@ -1774,24 +1537,24 @@
         <v>29.7</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O4" s="8">
         <v>46046</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1">
         <v>2024</v>
@@ -1800,16 +1563,16 @@
         <v>2024</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K5" s="1">
         <v>42</v>
@@ -1818,24 +1581,24 @@
         <v>29.7</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O5" s="8">
         <v>46046</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1">
         <v>2024</v>
@@ -1844,16 +1607,16 @@
         <v>2024</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K6" s="1">
         <v>42</v>
@@ -1862,24 +1625,24 @@
         <v>29.7</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O6" s="8">
         <v>46046</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1">
         <v>2024</v>
@@ -1888,16 +1651,16 @@
         <v>2024</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K7" s="1">
         <v>42</v>
@@ -1906,24 +1669,24 @@
         <v>29.7</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O7" s="8">
         <v>46046</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D8" s="1">
         <v>2024</v>
@@ -1932,16 +1695,16 @@
         <v>2024</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K8" s="1">
         <v>42</v>
@@ -1950,24 +1713,24 @@
         <v>29.7</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O8" s="8">
         <v>46046</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1">
         <v>2024</v>
@@ -1976,16 +1739,16 @@
         <v>2024</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K9" s="1">
         <v>42</v>
@@ -1994,24 +1757,24 @@
         <v>29.7</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O9" s="8">
         <v>46046</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1">
         <v>2024</v>
@@ -2020,16 +1783,16 @@
         <v>2024</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K10" s="1">
         <v>42</v>
@@ -2038,24 +1801,24 @@
         <v>29.7</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O10" s="8">
         <v>46046</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1">
         <v>2024</v>
@@ -2064,16 +1827,16 @@
         <v>2024</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K11" s="1">
         <v>42</v>
@@ -2082,24 +1845,24 @@
         <v>29.7</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O11" s="8">
         <v>46046</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="D12" s="1">
         <v>2024</v>
@@ -2108,16 +1871,16 @@
         <v>2024</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K12" s="1">
         <v>42</v>
@@ -2126,24 +1889,24 @@
         <v>29.7</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O12" s="8">
         <v>46046</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="D13" s="1">
         <v>2024</v>
@@ -2152,16 +1915,16 @@
         <v>2024</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K13" s="1">
         <v>42</v>
@@ -2170,24 +1933,24 @@
         <v>29.7</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O13" s="8">
         <v>46046</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1">
         <v>2024</v>
@@ -2196,16 +1959,16 @@
         <v>2024</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K14" s="1">
         <v>42</v>
@@ -2214,24 +1977,24 @@
         <v>29.7</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O14" s="8">
         <v>46046</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1">
         <v>2024</v>
@@ -2240,16 +2003,16 @@
         <v>2024</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K15" s="1">
         <v>42</v>
@@ -2258,24 +2021,24 @@
         <v>29.7</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O15" s="8">
         <v>46046</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1">
         <v>2024</v>
@@ -2284,16 +2047,16 @@
         <v>2024</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K16" s="1">
         <v>42</v>
@@ -2302,24 +2065,24 @@
         <v>29.7</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O16" s="8">
         <v>46046</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D17" s="1">
         <v>2024</v>
@@ -2328,16 +2091,16 @@
         <v>2024</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K17" s="1">
         <v>42</v>
@@ -2346,24 +2109,24 @@
         <v>29.7</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O17" s="8">
         <v>46046</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D18" s="1">
         <v>2024</v>
@@ -2372,16 +2135,16 @@
         <v>2024</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K18" s="1">
         <v>42</v>
@@ -2390,24 +2153,24 @@
         <v>29.7</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O18" s="8">
         <v>46046</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1">
         <v>2024</v>
@@ -2416,16 +2179,16 @@
         <v>2024</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K19" s="1">
         <v>42</v>
@@ -2434,24 +2197,24 @@
         <v>29.7</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O19" s="8">
         <v>46046</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1">
         <v>2024</v>
@@ -2460,16 +2223,16 @@
         <v>2024</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K20" s="1">
         <v>42</v>
@@ -2478,24 +2241,24 @@
         <v>29.7</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O20" s="8">
         <v>46046</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D21" s="1">
         <v>2024</v>
@@ -2504,16 +2267,16 @@
         <v>2024</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K21" s="1">
         <v>42</v>
@@ -2522,24 +2285,24 @@
         <v>29.7</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O21" s="8">
         <v>46046</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1">
         <v>2024</v>
@@ -2548,16 +2311,16 @@
         <v>2024</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K22" s="1">
         <v>42</v>
@@ -2566,24 +2329,24 @@
         <v>29.7</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O22" s="8">
         <v>46046</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1">
         <v>2024</v>
@@ -2592,16 +2355,16 @@
         <v>2024</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K23" s="1">
         <v>42</v>
@@ -2610,24 +2373,24 @@
         <v>29.7</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O23" s="8">
         <v>46046</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D24" s="1">
         <v>2024</v>
@@ -2636,16 +2399,16 @@
         <v>2024</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K24" s="1">
         <v>42</v>
@@ -2654,24 +2417,24 @@
         <v>29.7</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O24" s="8">
         <v>46046</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="D25" s="1">
         <v>2024</v>
@@ -2680,16 +2443,16 @@
         <v>2024</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K25" s="1">
         <v>42</v>
@@ -2698,24 +2461,24 @@
         <v>29.7</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O25" s="8">
         <v>46046</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D26" s="1">
         <v>2024</v>
@@ -2724,16 +2487,16 @@
         <v>2024</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K26" s="1">
         <v>42</v>
@@ -2742,24 +2505,24 @@
         <v>29.7</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O26" s="8">
         <v>46046</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D27" s="1">
         <v>2024</v>
@@ -2768,16 +2531,16 @@
         <v>2024</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K27" s="1">
         <v>42</v>
@@ -2786,24 +2549,24 @@
         <v>29.7</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O27" s="8">
         <v>46046</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D28" s="1">
         <v>2024</v>
@@ -2812,16 +2575,16 @@
         <v>2024</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K28" s="1">
         <v>42</v>
@@ -2830,24 +2593,24 @@
         <v>29.7</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O28" s="8">
         <v>46046</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D29" s="1">
         <v>2024</v>
@@ -2856,16 +2619,16 @@
         <v>2024</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K29" s="1">
         <v>42</v>
@@ -2874,24 +2637,24 @@
         <v>29.7</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O29" s="8">
         <v>46046</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D30" s="1">
         <v>2024</v>
@@ -2900,16 +2663,16 @@
         <v>2024</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K30" s="1">
         <v>42</v>
@@ -2918,24 +2681,24 @@
         <v>29.7</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O30" s="8">
         <v>46046</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D31" s="1">
         <v>2024</v>
@@ -2944,16 +2707,16 @@
         <v>2024</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K31" s="1">
         <v>42</v>
@@ -2962,24 +2725,24 @@
         <v>29.7</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O31" s="8">
         <v>46046</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D32" s="1">
         <v>2024</v>
@@ -2988,16 +2751,16 @@
         <v>2024</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K32" s="1">
         <v>42</v>
@@ -3006,24 +2769,24 @@
         <v>29.7</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O32" s="8">
         <v>46046</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D33" s="1">
         <v>2024</v>
@@ -3032,16 +2795,16 @@
         <v>2024</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K33" s="1">
         <v>42</v>
@@ -3050,24 +2813,24 @@
         <v>29.7</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O33" s="8">
         <v>46046</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D34" s="1">
         <v>2024</v>
@@ -3076,16 +2839,16 @@
         <v>2024</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K34" s="1">
         <v>42</v>
@@ -3094,24 +2857,24 @@
         <v>29.7</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O34" s="8">
         <v>46046</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="D35" s="1">
         <v>2024</v>
@@ -3120,16 +2883,16 @@
         <v>2024</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K35" s="1">
         <v>42</v>
@@ -3138,24 +2901,24 @@
         <v>29.7</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O35" s="8">
         <v>46046</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="D36" s="1">
         <v>2024</v>
@@ -3164,16 +2927,16 @@
         <v>2024</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K36" s="1">
         <v>42</v>
@@ -3182,24 +2945,24 @@
         <v>29.7</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O36" s="8">
         <v>46046</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D37" s="1">
         <v>2024</v>
@@ -3208,16 +2971,16 @@
         <v>2024</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K37" s="1">
         <v>42</v>
@@ -3226,24 +2989,24 @@
         <v>29.7</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O37" s="8">
         <v>46046</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D38" s="1">
         <v>2024</v>
@@ -3252,16 +3015,16 @@
         <v>2024</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K38" s="1">
         <v>42</v>
@@ -3270,24 +3033,24 @@
         <v>29.7</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O38" s="8">
         <v>46046</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D39" s="1">
         <v>2024</v>
@@ -3296,16 +3059,16 @@
         <v>2024</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K39" s="1">
         <v>42</v>
@@ -3314,24 +3077,24 @@
         <v>29.7</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O39" s="8">
         <v>46046</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D40" s="1">
         <v>2024</v>
@@ -3340,16 +3103,16 @@
         <v>2024</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K40" s="1">
         <v>42</v>
@@ -3358,24 +3121,24 @@
         <v>29.7</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O40" s="8">
         <v>46046</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D41" s="1">
         <v>2024</v>
@@ -3384,16 +3147,16 @@
         <v>2024</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K41" s="1">
         <v>42</v>
@@ -3402,24 +3165,24 @@
         <v>29.7</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O41" s="8">
         <v>46046</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D42" s="1">
         <v>2024</v>
@@ -3428,16 +3191,16 @@
         <v>2024</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K42" s="1">
         <v>42</v>
@@ -3446,24 +3209,24 @@
         <v>29.7</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O42" s="8">
         <v>46046</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D43" s="1">
         <v>2024</v>
@@ -3472,16 +3235,16 @@
         <v>2024</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K43" s="1">
         <v>42</v>
@@ -3490,24 +3253,24 @@
         <v>29.7</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O43" s="8">
         <v>46046</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D44" s="1">
         <v>2024</v>
@@ -3516,16 +3279,16 @@
         <v>2024</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K44" s="1">
         <v>42</v>
@@ -3534,24 +3297,24 @@
         <v>29.7</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O44" s="8">
         <v>46046</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D45" s="1">
         <v>2024</v>
@@ -3560,16 +3323,16 @@
         <v>2024</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K45" s="1">
         <v>42</v>
@@ -3578,24 +3341,24 @@
         <v>29.7</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O45" s="8">
         <v>46046</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D46" s="1">
         <v>2024</v>
@@ -3604,16 +3367,16 @@
         <v>2024</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K46" s="1">
         <v>42</v>
@@ -3622,24 +3385,24 @@
         <v>29.7</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O46" s="8">
         <v>46046</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D47" s="1">
         <v>2024</v>
@@ -3648,16 +3411,16 @@
         <v>2024</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K47" s="1">
         <v>42</v>
@@ -3666,24 +3429,24 @@
         <v>29.7</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O47" s="8">
         <v>46046</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D48" s="1">
         <v>2024</v>
@@ -3692,16 +3455,16 @@
         <v>2024</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K48" s="1">
         <v>42</v>
@@ -3710,24 +3473,24 @@
         <v>29.7</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O48" s="8">
         <v>46046</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D49" s="1">
         <v>2024</v>
@@ -3736,16 +3499,16 @@
         <v>2024</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K49" s="1">
         <v>42</v>
@@ -3754,24 +3517,24 @@
         <v>29.7</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O49" s="8">
         <v>46046</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D50" s="1">
         <v>2024</v>
@@ -3780,16 +3543,16 @@
         <v>2024</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K50" s="1">
         <v>42</v>
@@ -3798,24 +3561,24 @@
         <v>29.7</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O50" s="8">
         <v>46046</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D51" s="1">
         <v>2024</v>
@@ -3824,16 +3587,16 @@
         <v>2024</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K51" s="1">
         <v>42</v>
@@ -3842,24 +3605,24 @@
         <v>29.7</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O51" s="8">
         <v>46046</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D52" s="1">
         <v>2024</v>
@@ -3868,16 +3631,16 @@
         <v>2024</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K52" s="1">
         <v>42</v>
@@ -3886,24 +3649,24 @@
         <v>29.7</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O52" s="8">
         <v>46046</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D53" s="1">
         <v>2024</v>
@@ -3912,16 +3675,16 @@
         <v>2024</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K53" s="1">
         <v>42</v>
@@ -3930,24 +3693,24 @@
         <v>29.7</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O53" s="8">
         <v>46046</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D54" s="1">
         <v>2024</v>
@@ -3956,16 +3719,16 @@
         <v>2024</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K54" s="1">
         <v>42</v>
@@ -3974,24 +3737,24 @@
         <v>29.7</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O54" s="8">
         <v>46046</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D55" s="1">
         <v>2024</v>
@@ -4000,16 +3763,16 @@
         <v>2024</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K55" s="1">
         <v>42</v>
@@ -4018,24 +3781,24 @@
         <v>29.7</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O55" s="8">
         <v>46046</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D56" s="1">
         <v>2024</v>
@@ -4044,16 +3807,16 @@
         <v>2024</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="K56" s="1">
         <v>42</v>
@@ -4062,13 +3825,13 @@
         <v>29.7</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="O56" s="8">
         <v>46046</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -4080,7 +3843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FD9C38-EEDE-3B48-B7E6-A7692F053C8D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -4096,21 +3859,21 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -4119,55 +3882,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A307C2-25E9-AF4C-9C45-B37330E6C0EA}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9B8475-BE87-C444-A643-36F19988A384}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4189,30 +3903,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>186</v>
+        <v>153</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C2" s="6">
         <v>2025</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4220,7 +3934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8090762-04EB-FC46-90C1-9A8DE33FBED9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4240,21 +3954,21 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8">
         <v>46051</v>
@@ -4266,7 +3980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D2348F-09E6-1C4F-A712-D75D02A09D8F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4286,55 +4000,18 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC30609-FE54-1C46-AE81-1F762FADE82A}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="31.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added found forms works
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C66F62-7030-FF49-BC08-61561DB7E96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FA6616-13A6-254E-BCB1-176AD165083E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
@@ -856,9 +856,6 @@
     <t>found form 13 (mother and child).jpg</t>
   </si>
   <si>
-    <t>draft</t>
-  </si>
-  <si>
     <t>found form (2017-06-29)</t>
   </si>
   <si>
@@ -1175,6 +1172,9 @@
   </si>
   <si>
     <t>forms</t>
+  </si>
+  <si>
+    <t>ready</t>
   </si>
 </sst>
 </file>
@@ -1594,7 +1594,7 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2054,11 +2054,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A006D3C4-93E9-0943-8732-0CF384DB2AB6}">
   <dimension ref="A1:X107"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1:L1048576"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -4912,13 +4912,13 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>260</v>
@@ -4933,13 +4933,13 @@
         <v>2017</v>
       </c>
       <c r="H57" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="J57" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L57" s="1">
         <v>30</v>
@@ -4948,7 +4948,7 @@
         <v>30</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P57" s="8">
         <v>46053</v>
@@ -4959,13 +4959,13 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>260</v>
@@ -4980,13 +4980,13 @@
         <v>2017</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I58" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L58" s="1">
         <v>30</v>
@@ -4995,7 +4995,7 @@
         <v>30</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P58" s="8">
         <v>46053</v>
@@ -5006,13 +5006,13 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>260</v>
@@ -5027,13 +5027,13 @@
         <v>2017</v>
       </c>
       <c r="H59" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="J59" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L59" s="1">
         <v>30</v>
@@ -5042,7 +5042,7 @@
         <v>30</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P59" s="8">
         <v>46053</v>
@@ -5053,13 +5053,13 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>260</v>
@@ -5074,13 +5074,13 @@
         <v>2017</v>
       </c>
       <c r="H60" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L60" s="1">
         <v>30</v>
@@ -5089,7 +5089,7 @@
         <v>30</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P60" s="8">
         <v>46053</v>
@@ -5100,13 +5100,13 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>260</v>
@@ -5121,13 +5121,13 @@
         <v>2024</v>
       </c>
       <c r="H61" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I61" s="1" t="s">
+      <c r="J61" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L61" s="1">
         <v>30</v>
@@ -5136,7 +5136,7 @@
         <v>40</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P61" s="8">
         <v>46053</v>
@@ -5147,13 +5147,13 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>260</v>
@@ -5168,13 +5168,13 @@
         <v>2024</v>
       </c>
       <c r="H62" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L62" s="1">
         <v>30</v>
@@ -5183,7 +5183,7 @@
         <v>30</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P62" s="8">
         <v>46053</v>
@@ -5194,13 +5194,13 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>260</v>
@@ -5215,13 +5215,13 @@
         <v>2024</v>
       </c>
       <c r="H63" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I63" s="1" t="s">
+      <c r="J63" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L63" s="1">
         <v>30</v>
@@ -5230,7 +5230,7 @@
         <v>30</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P63" s="8">
         <v>46053</v>
@@ -5241,13 +5241,13 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>260</v>
@@ -5262,13 +5262,13 @@
         <v>2025</v>
       </c>
       <c r="H64" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I64" s="1" t="s">
+      <c r="J64" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L64" s="1">
         <v>30</v>
@@ -5277,7 +5277,7 @@
         <v>40</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P64" s="8">
         <v>46053</v>
@@ -5288,13 +5288,13 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>260</v>
@@ -5309,13 +5309,13 @@
         <v>2025</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I65" s="1" t="s">
+      <c r="J65" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J65" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L65" s="1">
         <v>30</v>
@@ -5324,7 +5324,7 @@
         <v>30</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P65" s="8">
         <v>46053</v>
@@ -5335,13 +5335,13 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>260</v>
@@ -5356,13 +5356,13 @@
         <v>2025</v>
       </c>
       <c r="H66" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="J66" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L66" s="1">
         <v>40</v>
@@ -5371,7 +5371,7 @@
         <v>30</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P66" s="8">
         <v>46053</v>
@@ -5382,13 +5382,13 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>260</v>
@@ -5403,13 +5403,13 @@
         <v>2025</v>
       </c>
       <c r="H67" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I67" s="1" t="s">
+      <c r="J67" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J67" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L67" s="1">
         <v>30</v>
@@ -5418,7 +5418,7 @@
         <v>30</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P67" s="8">
         <v>46053</v>
@@ -5429,13 +5429,13 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>260</v>
@@ -5450,13 +5450,13 @@
         <v>2025</v>
       </c>
       <c r="H68" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I68" s="1" t="s">
+      <c r="J68" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L68" s="1">
         <v>30</v>
@@ -5465,7 +5465,7 @@
         <v>30</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P68" s="8">
         <v>46053</v>
@@ -5476,13 +5476,13 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>260</v>
@@ -5497,13 +5497,13 @@
         <v>2025</v>
       </c>
       <c r="H69" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="J69" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L69" s="1">
         <v>30</v>
@@ -5512,7 +5512,7 @@
         <v>30</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P69" s="8">
         <v>46053</v>
@@ -5523,13 +5523,13 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>260</v>
@@ -5544,13 +5544,13 @@
         <v>2024</v>
       </c>
       <c r="H70" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I70" s="1" t="s">
+      <c r="J70" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L70" s="1">
         <v>30</v>
@@ -5559,7 +5559,7 @@
         <v>30</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P70" s="8">
         <v>46053</v>
@@ -5570,13 +5570,13 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>260</v>
@@ -5591,22 +5591,22 @@
         <v>2024</v>
       </c>
       <c r="H71" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I71" s="1" t="s">
+      <c r="J71" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J71" s="1" t="s">
+      <c r="L71" s="1">
+        <v>50</v>
+      </c>
+      <c r="M71" s="1">
+        <v>50</v>
+      </c>
+      <c r="O71" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L71" s="1">
-        <v>50</v>
-      </c>
-      <c r="M71" s="1">
-        <v>50</v>
-      </c>
-      <c r="O71" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P71" s="8">
         <v>46053</v>
@@ -5617,13 +5617,13 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>260</v>
@@ -5638,22 +5638,22 @@
         <v>2024</v>
       </c>
       <c r="H72" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I72" s="1" t="s">
+      <c r="J72" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J72" s="1" t="s">
+      <c r="L72" s="1">
+        <v>50</v>
+      </c>
+      <c r="M72" s="1">
+        <v>50</v>
+      </c>
+      <c r="O72" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L72" s="1">
-        <v>50</v>
-      </c>
-      <c r="M72" s="1">
-        <v>50</v>
-      </c>
-      <c r="O72" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P72" s="8">
         <v>46053</v>
@@ -5664,13 +5664,13 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>260</v>
@@ -5685,22 +5685,22 @@
         <v>2024</v>
       </c>
       <c r="H73" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I73" s="1" t="s">
+      <c r="J73" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J73" s="1" t="s">
+      <c r="L73" s="1">
+        <v>50</v>
+      </c>
+      <c r="M73" s="1">
+        <v>50</v>
+      </c>
+      <c r="O73" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L73" s="1">
-        <v>50</v>
-      </c>
-      <c r="M73" s="1">
-        <v>50</v>
-      </c>
-      <c r="O73" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P73" s="8">
         <v>46053</v>
@@ -5711,13 +5711,13 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>260</v>
@@ -5732,22 +5732,22 @@
         <v>2024</v>
       </c>
       <c r="H74" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="J74" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="L74" s="1">
+        <v>50</v>
+      </c>
+      <c r="M74" s="1">
+        <v>50</v>
+      </c>
+      <c r="O74" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L74" s="1">
-        <v>50</v>
-      </c>
-      <c r="M74" s="1">
-        <v>50</v>
-      </c>
-      <c r="O74" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P74" s="8">
         <v>46053</v>
@@ -5758,13 +5758,13 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>260</v>
@@ -5779,22 +5779,22 @@
         <v>2024</v>
       </c>
       <c r="H75" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I75" s="1" t="s">
+      <c r="J75" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="L75" s="1">
+        <v>50</v>
+      </c>
+      <c r="M75" s="1">
+        <v>50</v>
+      </c>
+      <c r="O75" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L75" s="1">
-        <v>50</v>
-      </c>
-      <c r="M75" s="1">
-        <v>50</v>
-      </c>
-      <c r="O75" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P75" s="8">
         <v>46053</v>
@@ -5805,13 +5805,13 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>260</v>
@@ -5826,22 +5826,22 @@
         <v>2023</v>
       </c>
       <c r="H76" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I76" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J76" s="1" t="s">
+      <c r="L76" s="1">
+        <v>50</v>
+      </c>
+      <c r="M76" s="1">
+        <v>50</v>
+      </c>
+      <c r="O76" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L76" s="1">
-        <v>50</v>
-      </c>
-      <c r="M76" s="1">
-        <v>50</v>
-      </c>
-      <c r="O76" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P76" s="8">
         <v>46053</v>
@@ -5852,13 +5852,13 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>260</v>
@@ -5873,22 +5873,22 @@
         <v>2023</v>
       </c>
       <c r="H77" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I77" s="1" t="s">
+      <c r="J77" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J77" s="1" t="s">
+      <c r="L77" s="1">
+        <v>50</v>
+      </c>
+      <c r="M77" s="1">
+        <v>50</v>
+      </c>
+      <c r="O77" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L77" s="1">
-        <v>50</v>
-      </c>
-      <c r="M77" s="1">
-        <v>50</v>
-      </c>
-      <c r="O77" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P77" s="8">
         <v>46053</v>
@@ -5899,13 +5899,13 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>260</v>
@@ -5920,22 +5920,22 @@
         <v>2023</v>
       </c>
       <c r="H78" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I78" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I78" s="1" t="s">
+      <c r="J78" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J78" s="1" t="s">
+      <c r="L78" s="1">
+        <v>50</v>
+      </c>
+      <c r="M78" s="1">
+        <v>50</v>
+      </c>
+      <c r="O78" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L78" s="1">
-        <v>50</v>
-      </c>
-      <c r="M78" s="1">
-        <v>50</v>
-      </c>
-      <c r="O78" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P78" s="8">
         <v>46053</v>
@@ -5946,13 +5946,13 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>260</v>
@@ -5967,22 +5967,22 @@
         <v>2023</v>
       </c>
       <c r="H79" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I79" s="1" t="s">
+      <c r="J79" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J79" s="1" t="s">
+      <c r="L79" s="1">
+        <v>50</v>
+      </c>
+      <c r="M79" s="1">
+        <v>50</v>
+      </c>
+      <c r="O79" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L79" s="1">
-        <v>50</v>
-      </c>
-      <c r="M79" s="1">
-        <v>50</v>
-      </c>
-      <c r="O79" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P79" s="8">
         <v>46053</v>
@@ -5993,13 +5993,13 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>260</v>
@@ -6014,22 +6014,22 @@
         <v>2024</v>
       </c>
       <c r="H80" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I80" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I80" s="1" t="s">
+      <c r="J80" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J80" s="1" t="s">
+      <c r="L80" s="1">
+        <v>50</v>
+      </c>
+      <c r="M80" s="1">
+        <v>50</v>
+      </c>
+      <c r="O80" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="L80" s="1">
-        <v>50</v>
-      </c>
-      <c r="M80" s="1">
-        <v>50</v>
-      </c>
-      <c r="O80" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="P80" s="8">
         <v>46053</v>
@@ -6040,13 +6040,13 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>260</v>
@@ -6061,13 +6061,13 @@
         <v>2024</v>
       </c>
       <c r="H81" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I81" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I81" s="1" t="s">
+      <c r="J81" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J81" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L81" s="1">
         <v>40</v>
@@ -6076,7 +6076,7 @@
         <v>40</v>
       </c>
       <c r="O81" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P81" s="8">
         <v>46053</v>
@@ -6087,13 +6087,13 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>260</v>
@@ -6108,13 +6108,13 @@
         <v>2024</v>
       </c>
       <c r="H82" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I82" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I82" s="1" t="s">
+      <c r="J82" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J82" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L82" s="1">
         <v>40</v>
@@ -6123,7 +6123,7 @@
         <v>40</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P82" s="8">
         <v>46053</v>
@@ -6134,13 +6134,13 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>260</v>
@@ -6155,13 +6155,13 @@
         <v>2024</v>
       </c>
       <c r="H83" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I83" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I83" s="1" t="s">
+      <c r="J83" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L83" s="1">
         <v>40</v>
@@ -6170,7 +6170,7 @@
         <v>40</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P83" s="8">
         <v>46053</v>
@@ -6181,13 +6181,13 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>260</v>
@@ -6202,13 +6202,13 @@
         <v>2024</v>
       </c>
       <c r="H84" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I84" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I84" s="1" t="s">
+      <c r="J84" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J84" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L84" s="1">
         <v>30</v>
@@ -6217,7 +6217,7 @@
         <v>40</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P84" s="8">
         <v>46053</v>
@@ -6228,13 +6228,13 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>260</v>
@@ -6249,13 +6249,13 @@
         <v>2021</v>
       </c>
       <c r="H85" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I85" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I85" s="1" t="s">
+      <c r="J85" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J85" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L85" s="1">
         <v>30</v>
@@ -6264,7 +6264,7 @@
         <v>30</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P85" s="8">
         <v>46053</v>
@@ -6275,13 +6275,13 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>260</v>
@@ -6296,13 +6296,13 @@
         <v>2023</v>
       </c>
       <c r="H86" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I86" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I86" s="1" t="s">
+      <c r="J86" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L86" s="1">
         <v>30</v>
@@ -6311,7 +6311,7 @@
         <v>30</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P86" s="8">
         <v>46053</v>
@@ -6322,13 +6322,13 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>260</v>
@@ -6343,13 +6343,13 @@
         <v>2023</v>
       </c>
       <c r="H87" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I87" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I87" s="1" t="s">
+      <c r="J87" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L87" s="1">
         <v>30</v>
@@ -6358,7 +6358,7 @@
         <v>30</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P87" s="8">
         <v>46053</v>
@@ -6369,13 +6369,13 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>260</v>
@@ -6390,13 +6390,13 @@
         <v>2023</v>
       </c>
       <c r="H88" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I88" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I88" s="1" t="s">
+      <c r="J88" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J88" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L88" s="1">
         <v>30</v>
@@ -6405,7 +6405,7 @@
         <v>30</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P88" s="8">
         <v>46053</v>
@@ -6416,13 +6416,13 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>260</v>
@@ -6437,13 +6437,13 @@
         <v>2023</v>
       </c>
       <c r="H89" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I89" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I89" s="1" t="s">
+      <c r="J89" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J89" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L89" s="1">
         <v>30</v>
@@ -6452,7 +6452,7 @@
         <v>30</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P89" s="8">
         <v>46053</v>
@@ -6463,13 +6463,13 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>260</v>
@@ -6484,13 +6484,13 @@
         <v>2023</v>
       </c>
       <c r="H90" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I90" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I90" s="1" t="s">
+      <c r="J90" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J90" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L90" s="1">
         <v>30</v>
@@ -6499,7 +6499,7 @@
         <v>30</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P90" s="8">
         <v>46053</v>
@@ -6510,13 +6510,13 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>260</v>
@@ -6531,13 +6531,13 @@
         <v>2023</v>
       </c>
       <c r="H91" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I91" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I91" s="1" t="s">
+      <c r="J91" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J91" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L91" s="1">
         <v>30</v>
@@ -6546,7 +6546,7 @@
         <v>30</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P91" s="8">
         <v>46053</v>
@@ -6557,13 +6557,13 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>260</v>
@@ -6578,13 +6578,13 @@
         <v>2023</v>
       </c>
       <c r="H92" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I92" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I92" s="1" t="s">
+      <c r="J92" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J92" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L92" s="1">
         <v>30</v>
@@ -6593,7 +6593,7 @@
         <v>40</v>
       </c>
       <c r="O92" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P92" s="8">
         <v>46053</v>
@@ -6604,13 +6604,13 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>260</v>
@@ -6625,13 +6625,13 @@
         <v>2023</v>
       </c>
       <c r="H93" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I93" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I93" s="1" t="s">
+      <c r="J93" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L93" s="1">
         <v>30</v>
@@ -6640,7 +6640,7 @@
         <v>30</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P93" s="8">
         <v>46053</v>
@@ -6651,13 +6651,13 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>260</v>
@@ -6672,13 +6672,13 @@
         <v>2023</v>
       </c>
       <c r="H94" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I94" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I94" s="1" t="s">
+      <c r="J94" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J94" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L94" s="1">
         <v>22.5</v>
@@ -6687,7 +6687,7 @@
         <v>40</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P94" s="8">
         <v>46053</v>
@@ -6698,13 +6698,13 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>260</v>
@@ -6719,13 +6719,13 @@
         <v>2023</v>
       </c>
       <c r="H95" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I95" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I95" s="1" t="s">
+      <c r="J95" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J95" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L95" s="1">
         <v>22.5</v>
@@ -6734,7 +6734,7 @@
         <v>40</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P95" s="8">
         <v>46053</v>
@@ -6745,13 +6745,13 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>260</v>
@@ -6766,13 +6766,13 @@
         <v>2023</v>
       </c>
       <c r="H96" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I96" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I96" s="1" t="s">
+      <c r="J96" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J96" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L96" s="1">
         <v>30</v>
@@ -6781,7 +6781,7 @@
         <v>30</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P96" s="8">
         <v>46053</v>
@@ -6792,13 +6792,13 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>260</v>
@@ -6813,13 +6813,13 @@
         <v>2023</v>
       </c>
       <c r="H97" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I97" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I97" s="1" t="s">
+      <c r="J97" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J97" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L97" s="1">
         <v>30</v>
@@ -6828,7 +6828,7 @@
         <v>30</v>
       </c>
       <c r="O97" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P97" s="8">
         <v>46053</v>
@@ -6839,13 +6839,13 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>260</v>
@@ -6860,13 +6860,13 @@
         <v>2023</v>
       </c>
       <c r="H98" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I98" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I98" s="1" t="s">
+      <c r="J98" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J98" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L98" s="1">
         <v>30</v>
@@ -6875,7 +6875,7 @@
         <v>30</v>
       </c>
       <c r="O98" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P98" s="8">
         <v>46053</v>
@@ -6886,13 +6886,13 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>260</v>
@@ -6907,13 +6907,13 @@
         <v>2023</v>
       </c>
       <c r="H99" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I99" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I99" s="1" t="s">
+      <c r="J99" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J99" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L99" s="1">
         <v>30</v>
@@ -6922,7 +6922,7 @@
         <v>30</v>
       </c>
       <c r="O99" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P99" s="8">
         <v>46053</v>
@@ -6933,13 +6933,13 @@
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>260</v>
@@ -6954,13 +6954,13 @@
         <v>2023</v>
       </c>
       <c r="H100" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I100" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I100" s="1" t="s">
+      <c r="J100" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J100" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L100" s="1">
         <v>30</v>
@@ -6969,7 +6969,7 @@
         <v>30</v>
       </c>
       <c r="O100" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P100" s="8">
         <v>46053</v>
@@ -6980,13 +6980,13 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>260</v>
@@ -7001,13 +7001,13 @@
         <v>2023</v>
       </c>
       <c r="H101" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I101" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I101" s="1" t="s">
+      <c r="J101" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J101" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L101" s="1">
         <v>30</v>
@@ -7016,7 +7016,7 @@
         <v>30</v>
       </c>
       <c r="O101" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P101" s="8">
         <v>46053</v>
@@ -7027,13 +7027,13 @@
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>260</v>
@@ -7048,13 +7048,13 @@
         <v>2023</v>
       </c>
       <c r="H102" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I102" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I102" s="1" t="s">
+      <c r="J102" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J102" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L102" s="1">
         <v>30</v>
@@ -7063,7 +7063,7 @@
         <v>30</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P102" s="8">
         <v>46053</v>
@@ -7074,13 +7074,13 @@
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>260</v>
@@ -7095,13 +7095,13 @@
         <v>2023</v>
       </c>
       <c r="H103" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I103" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I103" s="1" t="s">
+      <c r="J103" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J103" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L103" s="1">
         <v>30</v>
@@ -7110,7 +7110,7 @@
         <v>30</v>
       </c>
       <c r="O103" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P103" s="8">
         <v>46053</v>
@@ -7121,13 +7121,13 @@
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>260</v>
@@ -7142,13 +7142,13 @@
         <v>2023</v>
       </c>
       <c r="H104" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I104" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I104" s="1" t="s">
+      <c r="J104" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J104" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L104" s="1">
         <v>40</v>
@@ -7157,7 +7157,7 @@
         <v>30</v>
       </c>
       <c r="O104" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P104" s="8">
         <v>46053</v>
@@ -7168,13 +7168,13 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>260</v>
@@ -7189,13 +7189,13 @@
         <v>2023</v>
       </c>
       <c r="H105" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I105" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I105" s="1" t="s">
+      <c r="J105" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L105" s="1">
         <v>30</v>
@@ -7204,7 +7204,7 @@
         <v>30</v>
       </c>
       <c r="O105" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P105" s="8">
         <v>46053</v>
@@ -7215,13 +7215,13 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>260</v>
@@ -7236,13 +7236,13 @@
         <v>2023</v>
       </c>
       <c r="H106" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I106" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I106" s="1" t="s">
+      <c r="J106" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J106" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L106" s="1">
         <v>30</v>
@@ -7251,7 +7251,7 @@
         <v>30</v>
       </c>
       <c r="O106" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P106" s="8">
         <v>46053</v>
@@ -7262,13 +7262,13 @@
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>271</v>
+        <v>377</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>260</v>
@@ -7283,13 +7283,13 @@
         <v>2023</v>
       </c>
       <c r="H107" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I107" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I107" s="1" t="s">
+      <c r="J107" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J107" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="L107" s="1">
         <v>30</v>
@@ -7298,7 +7298,7 @@
         <v>30</v>
       </c>
       <c r="O107" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P107" s="8">
         <v>46053</v>

</xml_diff>